<commit_message>
feat: working on uploading students exam scores
</commit_message>
<xml_diff>
--- a/excel_templates/register_students_template.xlsx
+++ b/excel_templates/register_students_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kev-powersoft\Documents\windows\marps\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,19 +370,20 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,6 +401,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5 E7:E1048576 E6">
+      <formula1>"M,F"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>